<commit_message>
Revision: add ANCOM-BC2 pattern analysis results
</commit_message>
<xml_diff>
--- a/results/outputs/urt_sim_summ_fixed.xlsx
+++ b/results/outputs/urt_sim_summ_fixed.xlsx
@@ -10,6 +10,7 @@
     <sheet name="bin" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="dunn" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="pair" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="trend" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -7212,4 +7213,778 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>165</v>
+      </c>
+      <c r="R1" t="s">
+        <v>166</v>
+      </c>
+      <c r="S1" t="s">
+        <v>170</v>
+      </c>
+      <c r="T1" t="s">
+        <v>171</v>
+      </c>
+      <c r="U1" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" t="s">
+        <v>201</v>
+      </c>
+      <c r="W1" t="s">
+        <v>204</v>
+      </c>
+      <c r="X1" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>217</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>241</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>256</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>